<commit_message>
chatbot interagindo com o usuário
</commit_message>
<xml_diff>
--- a/sentencas.xlsx
+++ b/sentencas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biaku\Documents\INSPER\7semestre\Processamento de Linguagem Natural\Chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729F6E9A-0E74-49BA-8705-3FC951107F0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B650C09-CFED-4D30-8152-142FAB646CEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9000" yWindow="4305" windowWidth="12840" windowHeight="8715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sentencas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="302">
   <si>
     <t>Intenção</t>
   </si>
@@ -623,6 +623,309 @@
   </si>
   <si>
     <t>Aumenta um pouco o ar condicionado</t>
+  </si>
+  <si>
+    <t>Não sei</t>
+  </si>
+  <si>
+    <t>Quais os meus compromissos de hoje?</t>
+  </si>
+  <si>
+    <t>Quanto foi o jogo do Palmeiras?</t>
+  </si>
+  <si>
+    <t>Foxbot, como faço para chegar em casa?</t>
+  </si>
+  <si>
+    <t>Hoje tem jogo do Barcelona?</t>
+  </si>
+  <si>
+    <t>Mostre uma foto do Neymar</t>
+  </si>
+  <si>
+    <t>mostre uma receita de caipirinha</t>
+  </si>
+  <si>
+    <t>Quem ganhou o último BBB?</t>
+  </si>
+  <si>
+    <t>Mostre a meus compromissos para a semana</t>
+  </si>
+  <si>
+    <t>Consulte o número de mortes por coronavírus hoje</t>
+  </si>
+  <si>
+    <t>O Palmeiras tem mundial?</t>
+  </si>
+  <si>
+    <t>Quando foi o último título do São Paulo?</t>
+  </si>
+  <si>
+    <t>Conte uma piada</t>
+  </si>
+  <si>
+    <t>Quem é a Gabi da AE4?</t>
+  </si>
+  <si>
+    <t>O Matheus é um autômato?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como faço para baixar RAM? </t>
+  </si>
+  <si>
+    <t>Marque uma consulta com o meu médico para semana que vem.</t>
+  </si>
+  <si>
+    <t>Você me ama?</t>
+  </si>
+  <si>
+    <t>Foxbot, qual a melhor rota para chegar em casa?</t>
+  </si>
+  <si>
+    <t>Como faço para aumentar meu pênis?</t>
+  </si>
+  <si>
+    <t>Por que o Ribamar não é da seleção?</t>
+  </si>
+  <si>
+    <t>Receita de miojo</t>
+  </si>
+  <si>
+    <t>De que cookie você gosta?</t>
+  </si>
+  <si>
+    <t>Você acredita em Deus?</t>
+  </si>
+  <si>
+    <t>Ainda tenho compromissos hoje?</t>
+  </si>
+  <si>
+    <t>Foxbot, o Acre existe?</t>
+  </si>
+  <si>
+    <t>Foxbot, toque Grupo Menos é Mais</t>
+  </si>
+  <si>
+    <t>Mostre fotos do carnaval passado</t>
+  </si>
+  <si>
+    <t>Vacina transforma em jacaré?</t>
+  </si>
+  <si>
+    <t>O que é um mamaco?</t>
+  </si>
+  <si>
+    <t>Marque uma reunião com o estagiário para amanhã as 17 horas</t>
+  </si>
+  <si>
+    <t>Por que não escovar os dentes com Hipoglós?</t>
+  </si>
+  <si>
+    <t>Foxbot, bora fumar um?</t>
+  </si>
+  <si>
+    <t>Foxbot, toque Thiaguinho</t>
+  </si>
+  <si>
+    <t>Foxbot, coloque um alarme para amanhã às 7h30</t>
+  </si>
+  <si>
+    <t>Me acorde amanhã às 9 horas</t>
+  </si>
+  <si>
+    <t>Malboro é um bom pré treino?</t>
+  </si>
+  <si>
+    <t>Foxbot, ligue o cronômetro</t>
+  </si>
+  <si>
+    <t>Foxbot, ligue para a maravilhosa</t>
+  </si>
+  <si>
+    <t>Abra a câmera</t>
+  </si>
+  <si>
+    <t>Foxbot, quantos banhos a Viih Tube toma por semana?</t>
+  </si>
+  <si>
+    <t>Foxbot, por que foram comer o morcego?</t>
+  </si>
+  <si>
+    <t>É necessário mexer o macarrão enquanto cozinha?</t>
+  </si>
+  <si>
+    <t>Procure vídeos do Ronaldinho</t>
+  </si>
+  <si>
+    <t>Como colocar uma camisinha?</t>
+  </si>
+  <si>
+    <t>Ligue um timer por 15 minutos</t>
+  </si>
+  <si>
+    <t>Quanto está o jogo do PSG?</t>
+  </si>
+  <si>
+    <t>Qual é o próximo compromisso do dia?</t>
+  </si>
+  <si>
+    <t>Foxbot, pare o cronômetro</t>
+  </si>
+  <si>
+    <t>Por que o Thiago Leifert parece um sapatênis?</t>
+  </si>
+  <si>
+    <t>O que fazer agora que acabou a água?</t>
+  </si>
+  <si>
+    <t>Baixar tinta de impressora</t>
+  </si>
+  <si>
+    <t>Tem alguma música ruim do Barões da Pisadinha?</t>
+  </si>
+  <si>
+    <t>Amor ou o litrão?</t>
+  </si>
+  <si>
+    <t>Quem é nóia é imune ao coronavírus?</t>
+  </si>
+  <si>
+    <t>Tutorial de como enganar um agiota</t>
+  </si>
+  <si>
+    <t>Como saber se ela gosta de mim?</t>
+  </si>
+  <si>
+    <t>Como ficar rico com daytrade?</t>
+  </si>
+  <si>
+    <t>O que é quarentena?</t>
+  </si>
+  <si>
+    <t>Foxbot, meu colesterol está alto?</t>
+  </si>
+  <si>
+    <t>Qual é o almoço de hoje?</t>
+  </si>
+  <si>
+    <t>Quanto custa uma Itubaína</t>
+  </si>
+  <si>
+    <t>Quantos anos vive uma lagosta?</t>
+  </si>
+  <si>
+    <t>Por que liga da justiça é ruim?</t>
+  </si>
+  <si>
+    <t>Mostre a nota de Corra no IMDB</t>
+  </si>
+  <si>
+    <t>Como prender a respiração?</t>
+  </si>
+  <si>
+    <t>Quando foi a última vez que tomei banho?</t>
+  </si>
+  <si>
+    <t>Por que existem pessoas que riem como porcos?</t>
+  </si>
+  <si>
+    <t>Onde encontro um dodo de estimação?</t>
+  </si>
+  <si>
+    <t>O que são mulheres-sapiens?</t>
+  </si>
+  <si>
+    <t>Postos de gasolina perto de mim</t>
+  </si>
+  <si>
+    <t>Quero um milkshake de ovomaltine</t>
+  </si>
+  <si>
+    <t>Por que curva de rio acumula lixo?</t>
+  </si>
+  <si>
+    <t>Foxbot, pare o timer</t>
+  </si>
+  <si>
+    <t>Mostre o meu próximo compromisso</t>
+  </si>
+  <si>
+    <t>Toque minha playlist de funk</t>
+  </si>
+  <si>
+    <t>O que é trap?</t>
+  </si>
+  <si>
+    <t>Quanto tempo o cronômetro está marcando?</t>
+  </si>
+  <si>
+    <t>Foxbot, me mostre uma receita de bolo</t>
+  </si>
+  <si>
+    <t>Quanto está custando uma ação da Cyrela?</t>
+  </si>
+  <si>
+    <t>Quem é Carlos Adão?</t>
+  </si>
+  <si>
+    <t>Qual o nome do gorila que morreu em 2016?</t>
+  </si>
+  <si>
+    <t>Como tratar queimaduras de sol?</t>
+  </si>
+  <si>
+    <t>Qual a altura máxima de um anão?</t>
+  </si>
+  <si>
+    <t>Diga a rota para o Maracanã</t>
+  </si>
+  <si>
+    <t>Coronavac engravida?</t>
+  </si>
+  <si>
+    <t>Como tá o câmbio de dólar pra real?</t>
+  </si>
+  <si>
+    <t>Como saber se fui hackeado?</t>
+  </si>
+  <si>
+    <t>Foxbot, marque dentista para amanhã às 10h</t>
+  </si>
+  <si>
+    <t>Foxbot, ligue a impressora</t>
+  </si>
+  <si>
+    <t>Foxbot, quantas calorias eu gastei hoje?</t>
+  </si>
+  <si>
+    <t>Foxbot, toque uma música de ambiente</t>
+  </si>
+  <si>
+    <t>Diminua o volume da música</t>
+  </si>
+  <si>
+    <t>Foxbot, reserve uma mesa no Varanda para as 19h.</t>
+  </si>
+  <si>
+    <t>Foxbot, acesse o site da Netshoes</t>
+  </si>
+  <si>
+    <t>Como se fala eu amo você em russo?</t>
+  </si>
+  <si>
+    <t>Foxbot, quando é o próximo show do Alok?</t>
+  </si>
+  <si>
+    <t>Onde fica o Taj Mahal?</t>
+  </si>
+  <si>
+    <t>Foxbot, quanto está uma passagem para Miami?</t>
+  </si>
+  <si>
+    <t>Foxbot, quantas calorias tem uma torta de limão?</t>
+  </si>
+  <si>
+    <t>Foxbot, mande uma mensagem para a minha irmã.</t>
   </si>
 </sst>
 </file>
@@ -658,7 +961,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -962,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B200"/>
+  <dimension ref="A1:B300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2574,6 +2878,806 @@
         <v>200</v>
       </c>
     </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>